<commit_message>
Chairs Per Carton sheet added
</commit_message>
<xml_diff>
--- a/Quick Ship Router/bin/Debug/Kanban Blank Color Cross Reference.xlsx
+++ b/Quick Ship Router/bin/Debug/Kanban Blank Color Cross Reference.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Gage Omega\Programming\Quick Ship Router\Quick Ship Router\bin\Debug\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Gage Omega\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7500" tabRatio="658" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7500" tabRatio="658" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Blank Summaries" sheetId="16" r:id="rId1"/>
@@ -38,10 +38,10 @@
   </definedNames>
   <calcPr calcId="152511"/>
   <pivotCaches>
-    <pivotCache cacheId="8" r:id="rId19"/>
-    <pivotCache cacheId="9" r:id="rId20"/>
-    <pivotCache cacheId="10" r:id="rId21"/>
-    <pivotCache cacheId="11" r:id="rId22"/>
+    <pivotCache cacheId="0" r:id="rId19"/>
+    <pivotCache cacheId="1" r:id="rId20"/>
+    <pivotCache cacheId="2" r:id="rId21"/>
+    <pivotCache cacheId="3" r:id="rId22"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -14681,7 +14681,213 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="11" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:F18" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="18">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="19">
+        <item m="1" x="4"/>
+        <item m="1" x="15"/>
+        <item m="1" x="6"/>
+        <item m="1" x="11"/>
+        <item m="1" x="10"/>
+        <item m="1" x="8"/>
+        <item m="1" x="7"/>
+        <item m="1" x="14"/>
+        <item m="1" x="16"/>
+        <item m="1" x="17"/>
+        <item m="1" x="5"/>
+        <item m="1" x="12"/>
+        <item m="1" x="9"/>
+        <item m="1" x="13"/>
+        <item x="1"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0" sortType="descending">
+      <items count="14">
+        <item x="12"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="0"/>
+        <item x="9"/>
+        <item x="7"/>
+        <item x="5"/>
+        <item x="2"/>
+        <item x="11"/>
+        <item x="1"/>
+        <item x="6"/>
+        <item x="10"/>
+        <item x="8"/>
+        <item t="default"/>
+      </items>
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
+    </pivotField>
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="3"/>
+  </rowFields>
+  <rowItems count="14">
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="2"/>
+  </colFields>
+  <colItems count="5">
+    <i>
+      <x v="14"/>
+    </i>
+    <i>
+      <x v="15"/>
+    </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Total" fld="17" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="6">
+    <format dxfId="9">
+      <pivotArea dataOnly="0" fieldPosition="0">
+        <references count="1">
+          <reference field="3" count="1">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="8">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="3" count="1">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="7">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="3" count="1">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="6">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="3" count="1">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="5">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="3" count="1">
+            <x v="9"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="4">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="3" count="1">
+            <x v="9"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="H8:I62" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="18">
     <pivotField showAll="0"/>
@@ -14925,214 +15131,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="11" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:F18" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="18">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisCol" showAll="0">
-      <items count="19">
-        <item m="1" x="4"/>
-        <item m="1" x="15"/>
-        <item m="1" x="6"/>
-        <item m="1" x="11"/>
-        <item m="1" x="10"/>
-        <item m="1" x="8"/>
-        <item m="1" x="7"/>
-        <item m="1" x="14"/>
-        <item m="1" x="16"/>
-        <item m="1" x="17"/>
-        <item m="1" x="5"/>
-        <item m="1" x="12"/>
-        <item m="1" x="9"/>
-        <item m="1" x="13"/>
-        <item x="1"/>
-        <item x="0"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0" sortType="descending">
-      <items count="14">
-        <item x="12"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="0"/>
-        <item x="9"/>
-        <item x="7"/>
-        <item x="5"/>
-        <item x="2"/>
-        <item x="11"/>
-        <item x="1"/>
-        <item x="6"/>
-        <item x="10"/>
-        <item x="8"/>
-        <item t="default"/>
-      </items>
-      <autoSortScope>
-        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
-          <references count="1">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </autoSortScope>
-    </pivotField>
-    <pivotField showAll="0" defaultSubtotal="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0" defaultSubtotal="0"/>
-    <pivotField showAll="0" defaultSubtotal="0"/>
-    <pivotField dataField="1" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="3"/>
-  </rowFields>
-  <rowItems count="14">
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="12"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="11"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="2"/>
-  </colFields>
-  <colItems count="5">
-    <i>
-      <x v="14"/>
-    </i>
-    <i>
-      <x v="15"/>
-    </i>
-    <i>
-      <x v="16"/>
-    </i>
-    <i>
-      <x v="17"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Sum of Total" fld="17" baseField="0" baseItem="0"/>
-  </dataFields>
-  <formats count="6">
-    <format dxfId="9">
-      <pivotArea dataOnly="0" fieldPosition="0">
-        <references count="1">
-          <reference field="3" count="1">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="8">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="3" count="1">
-            <x v="7"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="7">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="1">
-          <reference field="3" count="1">
-            <x v="7"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="6">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="3" count="1">
-            <x v="7"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="5">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="1">
-          <reference field="3" count="1">
-            <x v="9"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="4">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="3" count="1">
-            <x v="9"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable5" cacheId="11" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable5" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A1:B41" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="18">
     <pivotField axis="axisRow" showAll="0">
@@ -15346,7 +15346,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="10" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Data" updatedVersion="5" showMemberPropertyTips="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="1" indent="0" compact="0" compactData="0" gridDropZones="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="2" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Data" updatedVersion="5" showMemberPropertyTips="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="1" indent="0" compact="0" compactData="0" gridDropZones="1">
   <location ref="A3:B32" firstHeaderRow="2" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="14">
     <pivotField compact="0" outline="0" subtotalTop="0" showAll="0" includeNewItemsInFilter="1"/>
@@ -15504,7 +15504,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="10" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Data" updatedVersion="5" showMemberPropertyTips="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="1" indent="0" compact="0" compactData="0" gridDropZones="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="2" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Data" updatedVersion="5" showMemberPropertyTips="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="1" indent="0" compact="0" compactData="0" gridDropZones="1">
   <location ref="A3:B24" firstHeaderRow="2" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="14">
     <pivotField compact="0" outline="0" subtotalTop="0" showAll="0" includeNewItemsInFilter="1"/>
@@ -15630,7 +15630,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="9" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Data" updatedVersion="5" showMemberPropertyTips="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="1" indent="0" compact="0" compactData="0" gridDropZones="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="1" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Data" updatedVersion="5" showMemberPropertyTips="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="1" indent="0" compact="0" compactData="0" gridDropZones="1">
   <location ref="A3:B19" firstHeaderRow="2" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="15">
     <pivotField compact="0" outline="0" subtotalTop="0" showAll="0" includeNewItemsInFilter="1"/>
@@ -15742,7 +15742,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="9" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Data" updatedVersion="5" showMemberPropertyTips="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="1" indent="0" compact="0" compactData="0" gridDropZones="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="1" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Data" updatedVersion="5" showMemberPropertyTips="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="1" indent="0" compact="0" compactData="0" gridDropZones="1">
   <location ref="A3:B17" firstHeaderRow="2" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="15">
     <pivotField compact="0" outline="0" subtotalTop="0" showAll="0" includeNewItemsInFilter="1"/>
@@ -15841,7 +15841,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="8" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Data" updatedVersion="5" showMemberPropertyTips="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="1" indent="0" compact="0" compactData="0" gridDropZones="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Data" updatedVersion="5" showMemberPropertyTips="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="1" indent="0" compact="0" compactData="0" gridDropZones="1">
   <location ref="A3:B14" firstHeaderRow="2" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="15">
     <pivotField compact="0" outline="0" subtotalTop="0" showAll="0" includeNewItemsInFilter="1"/>
@@ -15933,7 +15933,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="8" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Data" updatedVersion="5" showMemberPropertyTips="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="1" indent="0" compact="0" compactData="0" gridDropZones="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="0" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Data" updatedVersion="5" showMemberPropertyTips="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="1" indent="0" compact="0" compactData="0" gridDropZones="1">
   <location ref="A3:B15" firstHeaderRow="2" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="15">
     <pivotField compact="0" outline="0" subtotalTop="0" showAll="0" includeNewItemsInFilter="1"/>
@@ -39776,7 +39776,7 @@
   </sheetPr>
   <dimension ref="A1:W77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>
@@ -41530,8 +41530,8 @@
   </sheetPr>
   <dimension ref="A1:AB86"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -41722,10 +41722,10 @@
         <v>702</v>
       </c>
       <c r="P3" s="124">
-        <v>41.75</v>
+        <v>40.25</v>
       </c>
       <c r="Q3" s="124">
-        <v>31.25</v>
+        <v>27.75</v>
       </c>
       <c r="R3" s="124">
         <v>2.5</v>
@@ -41832,11 +41832,11 @@
       <c r="B5" t="s">
         <v>561</v>
       </c>
-      <c r="C5" s="128">
-        <v>64.875</v>
-      </c>
-      <c r="D5" s="112">
-        <v>24.5</v>
+      <c r="C5" s="125">
+        <v>64.375</v>
+      </c>
+      <c r="D5" s="125">
+        <v>24</v>
       </c>
       <c r="E5" s="112">
         <v>2.5</v>
@@ -42813,10 +42813,10 @@
         <v>647</v>
       </c>
       <c r="P20" s="125">
-        <v>64.875</v>
+        <v>64.375</v>
       </c>
       <c r="Q20" s="125">
-        <v>24.5</v>
+        <v>24</v>
       </c>
       <c r="R20" s="125">
         <v>2.5</v>
@@ -43223,10 +43223,10 @@
         <v>652</v>
       </c>
       <c r="P27" s="125">
-        <v>64.88</v>
+        <v>63.25</v>
       </c>
       <c r="Q27" s="125">
-        <v>32</v>
+        <v>31.75</v>
       </c>
       <c r="R27" s="125">
         <v>2.5</v>
@@ -43359,10 +43359,10 @@
         <v>577</v>
       </c>
       <c r="C30" s="128">
-        <v>41.75</v>
+        <v>40.25</v>
       </c>
       <c r="D30" s="112">
-        <v>31.25</v>
+        <v>27.75</v>
       </c>
       <c r="E30" s="112">
         <v>2.5</v>
@@ -43649,18 +43649,18 @@
       <c r="L36" s="112"/>
       <c r="M36" s="112"/>
     </row>
-    <row r="37" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:28" ht="18" x14ac:dyDescent="0.2">
       <c r="A37" s="101" t="s">
         <v>488</v>
       </c>
       <c r="B37" t="s">
         <v>594</v>
       </c>
-      <c r="C37" s="128">
-        <v>64.875</v>
-      </c>
-      <c r="D37" s="112">
-        <v>24.5</v>
+      <c r="C37" s="125">
+        <v>64.375</v>
+      </c>
+      <c r="D37" s="125">
+        <v>24</v>
       </c>
       <c r="E37" s="112">
         <v>2.5</v>
@@ -44766,10 +44766,10 @@
         <v>557</v>
       </c>
       <c r="C74" s="128">
-        <v>64.88</v>
+        <v>63.25</v>
       </c>
       <c r="D74" s="112">
-        <v>32</v>
+        <v>31.75</v>
       </c>
       <c r="E74" s="112">
         <v>2.5</v>

</xml_diff>